<commit_message>
add jupyter notebook with data files
</commit_message>
<xml_diff>
--- a/data/incentive.xlsx
+++ b/data/incentive.xlsx
@@ -5,18 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kpikhtovnikov/Desktop/test/decision/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kpikhtovnikov/Desktop/test/decision/Bittensor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1995B2-5A37-EB42-8925-D8CEFFAECC52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17AEA02-2EAE-8F43-984F-04336A65635D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="520" windowWidth="25600" windowHeight="14280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1420" yWindow="2020" windowWidth="10000" windowHeight="11300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="122 miner" sheetId="1" r:id="rId1"/>
     <sheet name="203 miner" sheetId="2" r:id="rId2"/>
     <sheet name="221 miner" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'122 miner'!$C$1:$C$1814</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -16572,8 +16575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1814"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1048" workbookViewId="0">
-      <selection activeCell="B293" sqref="B293"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -36545,7 +36548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61BECB0-8981-6A4D-966F-A2FCB007EFBE}">
   <dimension ref="A1:C1584"/>
   <sheetViews>
-    <sheetView topLeftCell="A1050" workbookViewId="0">
+    <sheetView topLeftCell="A925" workbookViewId="0">
       <selection activeCell="E1130" sqref="E1130"/>
     </sheetView>
   </sheetViews>

</xml_diff>